<commit_message>
dynamic export by parses station_id
</commit_message>
<xml_diff>
--- a/api/data.xlsx
+++ b/api/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,161 +418,35 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>620610795</v>
+        <v>clbhmthk20000v4s4f4yu874a</v>
       </c>
       <c r="B2" t="str">
-        <v>clbgo28uj0002v47chxiqv7nf</v>
+        <v>clbgnzizb0000v4ag550yepfe</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>620610795</v>
+        <v>clbhmthk20000v4s4f4yu874a</v>
       </c>
       <c r="B3" t="str">
-        <v>clbhm8yef0000v4gchx39mhao</v>
+        <v>clbgnzizb0000v4ag550yepfe</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>620610795</v>
-      </c>
-      <c r="B4" t="str">
-        <v>clbhm8yef0000v4gchx39mhao</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>620610795</v>
-      </c>
-      <c r="B5" t="str">
-        <v>clbhm8yef0000v4gchx39mhao</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>620610795</v>
-      </c>
-      <c r="B6" t="str">
-        <v>clbhm8yef0000v4gchx39mhao</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>620610795</v>
-      </c>
-      <c r="B7" t="str">
-        <v>clbhm8yef0000v4gchx39mhao</v>
-      </c>
-      <c r="C7">
-        <v>11</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>620610795</v>
-      </c>
-      <c r="B8" t="str">
-        <v>clbhm8yef0000v4gchx39mhao</v>
-      </c>
-      <c r="C8">
-        <v>12</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>clbgnbwnk0000v49gc4vzxi30</v>
-      </c>
-      <c r="B9" t="str">
-        <v>clbhm8yef0000v4gchx39mhao</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>clbhmt8m70002v4osriw1o6qh</v>
-      </c>
-      <c r="B10" t="str">
-        <v>clbrq8zv10000v4qkm6zupibg</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>clbhmthk20000v4s4f4yu874a</v>
-      </c>
-      <c r="B11" t="str">
-        <v>clbgnzizb0000v4ag550yepfe</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>clbhmthk20000v4s4f4yu874a</v>
-      </c>
-      <c r="B12" t="str">
-        <v>clbgnzizb0000v4ag550yepfe</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>